<commit_message>
Foi adicionado um produto
</commit_message>
<xml_diff>
--- a/UNASPHT.xlsx
+++ b/UNASPHT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alciomar.hollanda\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alciomar.hollanda\Desktop\Alciomar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ESTOQUE" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>CODIGO</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Ricardo Eletro</t>
+  </si>
+  <si>
+    <t>Jodo da tia vera</t>
   </si>
 </sst>
 </file>
@@ -242,7 +245,37 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="36">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -254,20 +287,51 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="dd/mmm"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -286,31 +350,21 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="dd/mmm"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -329,21 +383,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -378,91 +417,10 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -481,6 +439,41 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -495,8 +488,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:F3" totalsRowShown="0" headerRowDxfId="26" dataDxfId="27">
-  <autoFilter ref="A1:F3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:F4" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:F4"/>
   <tableColumns count="6">
     <tableColumn id="1" name="CODIGO" dataDxfId="33"/>
     <tableColumn id="2" name="DESCRICAO" dataDxfId="32"/>
@@ -516,58 +509,58 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F5" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="35" tableBorderDxfId="36" totalsRowBorderDxfId="34">
-  <autoFilter ref="A1:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F6" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+  <autoFilter ref="A1:F6"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="9"/>
-    <tableColumn id="2" name="DESCRIÇÃO" dataDxfId="3">
+    <tableColumn id="1" name="ID" dataDxfId="23"/>
+    <tableColumn id="2" name="DESCRIÇÃO" dataDxfId="22">
       <calculatedColumnFormula>IF(A2="","",VLOOKUP(A2,ESTOQUE,2,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="VALOR" dataDxfId="8" dataCellStyle="Moeda">
+    <tableColumn id="3" name="VALOR" dataDxfId="21" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(A2="","",VLOOKUP(A2,ESTOQUE,3,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="DATA" dataDxfId="7"/>
-    <tableColumn id="5" name="QUANTIDADE" dataDxfId="6"/>
-    <tableColumn id="6" name="PESSOA" dataDxfId="5"/>
+    <tableColumn id="4" name="DATA" dataDxfId="20"/>
+    <tableColumn id="5" name="QUANTIDADE" dataDxfId="19"/>
+    <tableColumn id="6" name="PESSOA" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:F6" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:F6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:F6"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="25"/>
-    <tableColumn id="2" name="DESCRICAO" dataDxfId="24">
+    <tableColumn id="1" name="ID" dataDxfId="15"/>
+    <tableColumn id="2" name="DESCRICAO" dataDxfId="14">
       <calculatedColumnFormula>IF(A2="","",VLOOKUP(A2,ESTOQUE,2,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="VALOR" dataDxfId="23" dataCellStyle="Moeda">
+    <tableColumn id="3" name="VALOR" dataDxfId="13" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(B2="","",VLOOKUP(A2,ESTOQUE,3,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="DATA" dataDxfId="22"/>
-    <tableColumn id="5" name="SAIDA" dataDxfId="21"/>
-    <tableColumn id="6" name="PESSOA" dataDxfId="20"/>
+    <tableColumn id="4" name="DATA" dataDxfId="12"/>
+    <tableColumn id="5" name="SAIDA" dataDxfId="11"/>
+    <tableColumn id="6" name="PESSOA" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="T_PESSOA" displayName="T_PESSOA" ref="A1:G5" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="T_PESSOA" displayName="T_PESSOA" ref="A1:G5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G5"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="COD" dataDxfId="17"/>
-    <tableColumn id="2" name="NOME" dataDxfId="16"/>
-    <tableColumn id="3" name="IDADE" dataDxfId="15"/>
-    <tableColumn id="4" name="TELEFONE" dataDxfId="14"/>
-    <tableColumn id="5" name="ENTRADA" dataDxfId="13">
+    <tableColumn id="1" name="COD" dataDxfId="6"/>
+    <tableColumn id="2" name="NOME" dataDxfId="5"/>
+    <tableColumn id="3" name="IDADE" dataDxfId="4"/>
+    <tableColumn id="4" name="TELEFONE" dataDxfId="3"/>
+    <tableColumn id="5" name="ENTRADA" dataDxfId="2">
       <calculatedColumnFormula>SUMIF(ENTRADA!F:F,T_PESSOA[[#This Row],[NOME]],COD_QUANTIDADE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="SAIDA" dataDxfId="12">
+    <tableColumn id="6" name="SAIDA" dataDxfId="1">
       <calculatedColumnFormula>SUMIF(SAIDA!F:F,T_PESSOA[[#This Row],[NOME]],COD_QUANTIDADE_SAIDA)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="TOTAL" dataDxfId="2">
+    <tableColumn id="7" name="TOTAL" dataDxfId="0">
       <calculatedColumnFormula>T_PESSOA[[#This Row],[ENTRADA]]-T_PESSOA[[#This Row],[SAIDA]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -841,7 +834,7 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,6 +914,29 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <f>IF(A4="","",SUMIF(COD_ENTRADA,COD_ESTOQUE,COD_QUANTIDADE))</f>
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <f>IF(A4="","",SUMIF(COD_SAIDA,COD_ESTOQUE,COD_QUANTIDADE_SAIDA))</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <f>IF(D4="","",D4-E4)</f>
+        <v>10</v>
+      </c>
+    </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -931,7 +947,7 @@
         <v/>
       </c>
       <c r="F11" s="1" t="str">
-        <f t="shared" ref="F3:F66" si="2">IF(D11="","",D11-E11)</f>
+        <f t="shared" ref="F11:F66" si="2">IF(D11="","",D11-E11)</f>
         <v/>
       </c>
     </row>
@@ -1828,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1870,11 +1886,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="str">
-        <f t="shared" ref="B2:B19" si="0">IF(A2="","",VLOOKUP(A2,ESTOQUE,2,0))</f>
+        <f t="shared" ref="B2" si="0">IF(A2="","",VLOOKUP(A2,ESTOQUE,2,0))</f>
         <v>Xadrez</v>
       </c>
       <c r="C2" s="10">
-        <f t="shared" ref="C2:C13" si="1">IF(A2="","",VLOOKUP(A2,ESTOQUE,3,0))</f>
+        <f t="shared" ref="C2" si="1">IF(A2="","",VLOOKUP(A2,ESTOQUE,3,0))</f>
         <v>50</v>
       </c>
       <c r="D2" s="11">
@@ -1951,6 +1967,28 @@
       </c>
       <c r="F5" s="4" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="str">
+        <f>IF(A6="","",VLOOKUP(A6,ESTOQUE,2,0))</f>
+        <v>Jodo da tia vera</v>
+      </c>
+      <c r="C6" s="9">
+        <f>IF(A6="","",VLOOKUP(A6,ESTOQUE,3,0))</f>
+        <v>15</v>
+      </c>
+      <c r="D6" s="7">
+        <v>42862</v>
+      </c>
+      <c r="E6" s="8">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1966,7 +2004,7 @@
           <x14:formula1>
             <xm:f>PESSOA!$B:$B</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F5</xm:sqref>
+          <xm:sqref>F2:F6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2230,7 +2268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2283,7 +2321,7 @@
       </c>
       <c r="E2" s="1">
         <f>SUMIF(ENTRADA!F:F,T_PESSOA[[#This Row],[NOME]],COD_QUANTIDADE)</f>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1">
         <f>SUMIF(SAIDA!F:F,T_PESSOA[[#This Row],[NOME]],COD_QUANTIDADE_SAIDA)</f>
@@ -2291,7 +2329,7 @@
       </c>
       <c r="G2" s="1">
         <f>T_PESSOA[[#This Row],[ENTRADA]]-T_PESSOA[[#This Row],[SAIDA]]</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2365,7 +2403,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>